<commit_message>
add peer review tables
add peer review tables
</commit_message>
<xml_diff>
--- a/Documents/Foodies_PR.xlsx
+++ b/Documents/Foodies_PR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="6">
   <si>
     <t>publisher notes</t>
   </si>
@@ -42,10 +42,10 @@
     <t>Document Version</t>
   </si>
   <si>
-    <t>RTM-ID</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Document ID</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,343 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="120">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -141,15 +477,225 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="117"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="116"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="115"/>
+    <tableColumn id="4" name="Notes" dataDxfId="114"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="113"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="112"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1312" displayName="Table1312" ref="A3:F5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="45"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="44"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="43"/>
+    <tableColumn id="4" name="Notes" dataDxfId="42"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="41"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A3:F5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="37"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="36"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="35"/>
+    <tableColumn id="4" name="Notes" dataDxfId="34"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="33"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1314" displayName="Table1314" ref="A3:F5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="29"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="28"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="27"/>
+    <tableColumn id="4" name="Notes" dataDxfId="26"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="25"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A3:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="21"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="20"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="19"/>
+    <tableColumn id="4" name="Notes" dataDxfId="18"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="17"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table1316" displayName="Table1316" ref="A3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="13"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="12"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="11"/>
+    <tableColumn id="4" name="Notes" dataDxfId="10"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="9"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1317" displayName="Table1317" ref="A3:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="RTM-ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="4"/>
     <tableColumn id="3" name="Document Version" dataDxfId="3"/>
     <tableColumn id="4" name="Notes" dataDxfId="2"/>
     <tableColumn id="5" name="Reviewer Name" dataDxfId="1"/>
     <tableColumn id="6" name="publisher notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A3:F5" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="109"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="108"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="107"/>
+    <tableColumn id="4" name="Notes" dataDxfId="106"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="105"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="104"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A3:F5" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="101"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="100"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="99"/>
+    <tableColumn id="4" name="Notes" dataDxfId="98"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="97"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="96"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A3:F5" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="93"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="92"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="91"/>
+    <tableColumn id="4" name="Notes" dataDxfId="90"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="89"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="88"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A3:F5" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="85"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="84"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="83"/>
+    <tableColumn id="4" name="Notes" dataDxfId="82"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="81"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="80"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table138" displayName="Table138" ref="A3:F5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="77"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="76"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="75"/>
+    <tableColumn id="4" name="Notes" dataDxfId="74"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="73"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="72"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table139" displayName="Table139" ref="A3:F5" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="69"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="68"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="67"/>
+    <tableColumn id="4" name="Notes" dataDxfId="66"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="65"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="64"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1310" displayName="Table1310" ref="A3:F5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="61"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="60"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="59"/>
+    <tableColumn id="4" name="Notes" dataDxfId="58"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="57"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1311" displayName="Table1311" ref="A3:F5" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="53"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="52"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="51"/>
+    <tableColumn id="4" name="Notes" dataDxfId="50"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="49"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -444,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +1005,10 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -503,170 +1049,756 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add a review on SDD
add a review on use case diagram on SDD file
</commit_message>
<xml_diff>
--- a/Documents/Foodies_PR.xlsx
+++ b/Documents/Foodies_PR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="DefectReport" sheetId="13" r:id="rId13"/>
     <sheet name="TestCaseReport" sheetId="14" r:id="rId14"/>
     <sheet name="IssuesList" sheetId="15" r:id="rId15"/>
+    <sheet name="SDD" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="18">
   <si>
     <t>publisher notes</t>
   </si>
@@ -46,6 +47,42 @@
   </si>
   <si>
     <t>Document ID</t>
+  </si>
+  <si>
+    <t>PR_SDD_001</t>
+  </si>
+  <si>
+    <t>Foodies_Sys_UseCase_001</t>
+  </si>
+  <si>
+    <t>confirmation password is missing at steps number 2</t>
+  </si>
+  <si>
+    <t>Mariam Nesiem</t>
+  </si>
+  <si>
+    <t>PR_SDD_002</t>
+  </si>
+  <si>
+    <t>PR_SDD_003</t>
+  </si>
+  <si>
+    <t>PR_SDD_004</t>
+  </si>
+  <si>
+    <t>Foodies_Sys_UseCase_002</t>
+  </si>
+  <si>
+    <t>Foodies_Sys_UseCase_003</t>
+  </si>
+  <si>
+    <t>step number 4 from steps : system should return to home page not login page</t>
+  </si>
+  <si>
+    <t>step number 3.1 from steps : if user is an admin should be  redirected to admin panel not profiles page</t>
+  </si>
+  <si>
+    <t>step number 1 from steps : user can show loyalty points from user account page</t>
   </si>
 </sst>
 </file>
@@ -87,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -98,11 +135,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="128">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -477,7 +541,127 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="125"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="124"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="123"/>
+    <tableColumn id="4" name="Notes" dataDxfId="122"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="121"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="120"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1312" displayName="Table1312" ref="A3:F5" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="53"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="52"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="51"/>
+    <tableColumn id="4" name="Notes" dataDxfId="50"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="49"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="48"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A3:F5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="45"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="44"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="43"/>
+    <tableColumn id="4" name="Notes" dataDxfId="42"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="41"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1314" displayName="Table1314" ref="A3:F5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="37"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="36"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="35"/>
+    <tableColumn id="4" name="Notes" dataDxfId="34"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="33"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A3:F5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="29"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="28"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="27"/>
+    <tableColumn id="4" name="Notes" dataDxfId="26"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="25"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table1316" displayName="Table1316" ref="A3:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="21"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="20"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="19"/>
+    <tableColumn id="4" name="Notes" dataDxfId="18"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="17"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1317" displayName="Table1317" ref="A3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="13"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="12"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="11"/>
+    <tableColumn id="4" name="Notes" dataDxfId="10"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="9"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table13174" displayName="Table13174" ref="A3:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A3:F11"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="4"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="3"/>
+    <tableColumn id="4" name="Notes" dataDxfId="2"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="1"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A3:F5" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="117"/>
@@ -491,98 +675,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1312" displayName="Table1312" ref="A3:F5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="45"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="44"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="43"/>
-    <tableColumn id="4" name="Notes" dataDxfId="42"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="41"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="40"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A3:F5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="37"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="36"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="35"/>
-    <tableColumn id="4" name="Notes" dataDxfId="34"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="33"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="32"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1314" displayName="Table1314" ref="A3:F5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="29"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="28"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="27"/>
-    <tableColumn id="4" name="Notes" dataDxfId="26"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="25"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A3:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="21"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="20"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="19"/>
-    <tableColumn id="4" name="Notes" dataDxfId="18"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="17"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table1316" displayName="Table1316" ref="A3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="12"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="11"/>
-    <tableColumn id="4" name="Notes" dataDxfId="10"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="9"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1317" displayName="Table1317" ref="A3:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="4"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="3"/>
-    <tableColumn id="4" name="Notes" dataDxfId="2"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="1"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A3:F5" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A3:F5" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="109"/>
@@ -596,8 +690,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A3:F5" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A3:F5" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="101"/>
@@ -611,8 +705,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A3:F5" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A3:F5" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="93"/>
@@ -626,8 +720,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A3:F5" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table138" displayName="Table138" ref="A3:F5" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="85"/>
@@ -641,8 +735,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table138" displayName="Table138" ref="A3:F5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table139" displayName="Table139" ref="A3:F5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="77"/>
@@ -656,8 +750,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table139" displayName="Table139" ref="A3:F5" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1310" displayName="Table1310" ref="A3:F5" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="69"/>
@@ -671,8 +765,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1310" displayName="Table1310" ref="A3:F5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1311" displayName="Table1311" ref="A3:F5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="ID" dataDxfId="61"/>
@@ -681,21 +775,6 @@
     <tableColumn id="4" name="Notes" dataDxfId="58"/>
     <tableColumn id="5" name="Reviewer Name" dataDxfId="57"/>
     <tableColumn id="6" name="publisher notes" dataDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1311" displayName="Table1311" ref="A3:F5" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <autoFilter ref="A3:F5"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="53"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="52"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="51"/>
-    <tableColumn id="4" name="Notes" dataDxfId="50"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="49"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -990,7 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1371,6 +1450,156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F5"/>

</xml_diff>

<commit_message>
Peer Review Sheet updated
</commit_message>
<xml_diff>
--- a/Documents/Foodies_PR.xlsx
+++ b/Documents/Foodies_PR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="22">
   <si>
     <t>publisher notes</t>
   </si>
@@ -84,6 +84,18 @@
   <si>
     <t>step number 1 from steps : user can show loyalty points from user account page</t>
   </si>
+  <si>
+    <t>Date of finding</t>
+  </si>
+  <si>
+    <t>Date of Solving</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -138,11 +150,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="131">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -541,240 +565,243 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A3:F5" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="125"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="124"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="123"/>
-    <tableColumn id="4" name="Notes" dataDxfId="122"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="121"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="120"/>
+    <tableColumn id="1" name="ID" dataDxfId="128"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="127"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="126"/>
+    <tableColumn id="4" name="Notes" dataDxfId="125"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="124"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1312" displayName="Table1312" ref="A3:F5" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1312" displayName="Table1312" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="53"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="52"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="51"/>
-    <tableColumn id="4" name="Notes" dataDxfId="50"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="49"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="48"/>
+    <tableColumn id="1" name="ID" dataDxfId="56"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="55"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="54"/>
+    <tableColumn id="4" name="Notes" dataDxfId="53"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="52"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A3:F5" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A3:F5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="45"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="44"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="43"/>
-    <tableColumn id="4" name="Notes" dataDxfId="42"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="41"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="40"/>
+    <tableColumn id="1" name="ID" dataDxfId="48"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="47"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="46"/>
+    <tableColumn id="4" name="Notes" dataDxfId="45"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="44"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1314" displayName="Table1314" ref="A3:F5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table1314" displayName="Table1314" ref="A3:F5" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="37"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="36"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="35"/>
-    <tableColumn id="4" name="Notes" dataDxfId="34"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="33"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="32"/>
+    <tableColumn id="1" name="ID" dataDxfId="40"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="39"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="38"/>
+    <tableColumn id="4" name="Notes" dataDxfId="37"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="36"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A3:F5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1315" displayName="Table1315" ref="A3:F5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="29"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="28"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="27"/>
-    <tableColumn id="4" name="Notes" dataDxfId="26"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="25"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="24"/>
+    <tableColumn id="1" name="ID" dataDxfId="32"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="31"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="30"/>
+    <tableColumn id="4" name="Notes" dataDxfId="29"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="28"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table1316" displayName="Table1316" ref="A3:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table1316" displayName="Table1316" ref="A3:F5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="21"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="20"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="19"/>
-    <tableColumn id="4" name="Notes" dataDxfId="18"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="17"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="16"/>
+    <tableColumn id="1" name="ID" dataDxfId="24"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="23"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="22"/>
+    <tableColumn id="4" name="Notes" dataDxfId="21"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="20"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1317" displayName="Table1317" ref="A3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table1317" displayName="Table1317" ref="A3:F5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="12"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="11"/>
-    <tableColumn id="4" name="Notes" dataDxfId="10"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="9"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="8"/>
+    <tableColumn id="1" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="15"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="14"/>
+    <tableColumn id="4" name="Notes" dataDxfId="13"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="12"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table13174" displayName="Table13174" ref="A3:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A3:F11"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="4"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="3"/>
-    <tableColumn id="4" name="Notes" dataDxfId="2"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="1"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table13174" displayName="Table13174" ref="A3:I11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A3:I11"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="7"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="6"/>
+    <tableColumn id="4" name="Notes" dataDxfId="5"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="4"/>
+    <tableColumn id="9" name="Status" dataDxfId="0"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="3"/>
+    <tableColumn id="7" name="Date of finding" dataDxfId="2"/>
+    <tableColumn id="8" name="Date of Solving" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A3:F5" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A3:F5" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="117"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="116"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="115"/>
-    <tableColumn id="4" name="Notes" dataDxfId="114"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="113"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="112"/>
+    <tableColumn id="1" name="ID" dataDxfId="120"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="119"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="118"/>
+    <tableColumn id="4" name="Notes" dataDxfId="117"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="116"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A3:F5" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A3:F5" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="109"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="108"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="107"/>
-    <tableColumn id="4" name="Notes" dataDxfId="106"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="105"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="104"/>
+    <tableColumn id="1" name="ID" dataDxfId="112"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="111"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="110"/>
+    <tableColumn id="4" name="Notes" dataDxfId="109"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="108"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A3:F5" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A3:F5" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="101"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="100"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="99"/>
-    <tableColumn id="4" name="Notes" dataDxfId="98"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="97"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="96"/>
+    <tableColumn id="1" name="ID" dataDxfId="104"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="103"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="102"/>
+    <tableColumn id="4" name="Notes" dataDxfId="101"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="100"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A3:F5" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A3:F5" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="93"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="92"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="91"/>
-    <tableColumn id="4" name="Notes" dataDxfId="90"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="89"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="88"/>
+    <tableColumn id="1" name="ID" dataDxfId="96"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="95"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="94"/>
+    <tableColumn id="4" name="Notes" dataDxfId="93"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="92"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table138" displayName="Table138" ref="A3:F5" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table138" displayName="Table138" ref="A3:F5" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="85"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="84"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="83"/>
-    <tableColumn id="4" name="Notes" dataDxfId="82"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="81"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="80"/>
+    <tableColumn id="1" name="ID" dataDxfId="88"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="87"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="86"/>
+    <tableColumn id="4" name="Notes" dataDxfId="85"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="84"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table139" displayName="Table139" ref="A3:F5" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table139" displayName="Table139" ref="A3:F5" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="77"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="76"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="75"/>
-    <tableColumn id="4" name="Notes" dataDxfId="74"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="73"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="72"/>
+    <tableColumn id="1" name="ID" dataDxfId="80"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="79"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="78"/>
+    <tableColumn id="4" name="Notes" dataDxfId="77"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="76"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1310" displayName="Table1310" ref="A3:F5" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1310" displayName="Table1310" ref="A3:F5" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="69"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="68"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="67"/>
-    <tableColumn id="4" name="Notes" dataDxfId="66"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="65"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="64"/>
+    <tableColumn id="1" name="ID" dataDxfId="72"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="71"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="70"/>
+    <tableColumn id="4" name="Notes" dataDxfId="69"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="68"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1311" displayName="Table1311" ref="A3:F5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1311" displayName="Table1311" ref="A3:F5" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A3:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="61"/>
-    <tableColumn id="2" name="Document ID" dataDxfId="60"/>
-    <tableColumn id="3" name="Document Version" dataDxfId="59"/>
-    <tableColumn id="4" name="Notes" dataDxfId="58"/>
-    <tableColumn id="5" name="Reviewer Name" dataDxfId="57"/>
-    <tableColumn id="6" name="publisher notes" dataDxfId="56"/>
+    <tableColumn id="1" name="ID" dataDxfId="64"/>
+    <tableColumn id="2" name="Document ID" dataDxfId="63"/>
+    <tableColumn id="3" name="Document Version" dataDxfId="62"/>
+    <tableColumn id="4" name="Notes" dataDxfId="61"/>
+    <tableColumn id="5" name="Reviewer Name" dataDxfId="60"/>
+    <tableColumn id="6" name="publisher notes" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1073,16 +1100,16 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1102,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1110,7 +1137,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1134,9 +1161,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1164,7 +1191,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1188,9 +1215,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1210,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1218,7 +1245,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1242,9 +1269,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1264,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1272,7 +1299,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1296,9 +1323,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1318,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1326,7 +1353,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1350,9 +1377,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1372,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1380,7 +1407,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1404,9 +1431,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1434,7 +1461,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1452,23 +1479,25 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F11"/>
+  <dimension ref="A3:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1485,10 +1514,19 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1504,9 +1542,18 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="5">
+        <v>43713</v>
+      </c>
+      <c r="I4" s="5">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1522,9 +1569,18 @@
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="5">
+        <v>43713</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1540,9 +1596,18 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="5">
+        <v>43713</v>
+      </c>
+      <c r="I6" s="5">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1558,39 +1623,60 @@
       <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5">
+        <v>43713</v>
+      </c>
+      <c r="I7" s="5">
+        <v>43743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1608,9 +1694,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1630,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1638,7 +1724,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1662,9 +1748,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1692,7 +1778,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1716,9 +1802,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1738,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1746,7 +1832,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1770,9 +1856,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1792,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1800,7 +1886,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1824,9 +1910,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1846,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1854,7 +1940,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1878,9 +1964,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1900,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1908,7 +1994,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1932,9 +2018,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1962,7 +2048,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1986,9 +2072,9 @@
       <selection activeCell="A3" sqref="A3:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2008,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2016,7 +2102,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>